<commit_message>
Added dynamic search element
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/testData.xlsx
+++ b/src/main/java/TestData/testData.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2B702C7A-1373-489B-B64D-3C16FD4C57D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AC7A51C0-A336-40F9-BD99-DACBD3C41226}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:P7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -39,6 +40,15 @@
   </si>
   <si>
     <t>hey</t>
+  </si>
+  <si>
+    <t>Searchitem</t>
+  </si>
+  <si>
+    <t>65 inch tv Samsung</t>
+  </si>
+  <si>
+    <t>65 inch tv lg</t>
   </si>
 </sst>
 </file>
@@ -358,7 +368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -394,4 +404,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3049CFCF-2E3E-4174-B7A7-C47A6EEF1676}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modularized shopping cart class
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/testData.xlsx
+++ b/src/main/java/TestData/testData.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AC7A51C0-A336-40F9-BD99-DACBD3C41226}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\703177909\Git\src\main\java\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3068BD03-3366-4FC2-AB8F-46398E4E13CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,12 +34,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>rashrkp92@gmail.com</t>
-  </si>
-  <si>
-    <t>checkebay0!</t>
-  </si>
-  <si>
     <t>TestCaseName</t>
   </si>
   <si>
@@ -49,16 +47,30 @@
   </si>
   <si>
     <t>65 inch tv lg</t>
+  </si>
+  <si>
+    <t>audi.love25@gmail.com</t>
+  </si>
+  <si>
+    <t>Mitsubishi7!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +93,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -368,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,7 +396,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -392,16 +407,19 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F90622B5-2FB2-4F71-82E6-7CD67EEF60F4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -410,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3049CFCF-2E3E-4174-B7A7-C47A6EEF1676}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -421,17 +439,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>